<commit_message>
connected to IMU, set end of charge current, now also read battery status pin
</commit_message>
<xml_diff>
--- a/hardware/PCB/tstick-5gw-pro-USB-pcb/tstick-5gw-BOM.xlsx
+++ b/hardware/PCB/tstick-5gw-pro-USB-pcb/tstick-5gw-BOM.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Github\T-Stick\hardware\PCB\tstick-5gw-pro-USB-pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{8794FBB5-F1AA-437D-9E08-486770A8EDEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66608CDA-BFB9-4E78-A15B-290C7843C303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="4380" windowWidth="24240" windowHeight="13140"/>
+    <workbookView xWindow="28680" yWindow="4380" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tstick-5gw-pro-USB-BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="177">
   <si>
     <t>Qty</t>
   </si>
@@ -492,16 +505,77 @@
   </si>
   <si>
     <t>Total (CAD)</t>
+  </si>
+  <si>
+    <t>PCB Touch Board</t>
+  </si>
+  <si>
+    <t>Unit Price</t>
+  </si>
+  <si>
+    <t>Molex</t>
+  </si>
+  <si>
+    <t>541323262</t>
+  </si>
+  <si>
+    <t>Samtec Inc.</t>
+  </si>
+  <si>
+    <t>SSM-115-L-SV</t>
+  </si>
+  <si>
+    <t>SSM-106-L-SV</t>
+  </si>
+  <si>
+    <t>SM04B-SRSS-TB</t>
+  </si>
+  <si>
+    <t>TOUCH1, TOUCH2</t>
+  </si>
+  <si>
+    <t>TOUCH3</t>
+  </si>
+  <si>
+    <t>I2C1,I2C2,INT1,INT2</t>
+  </si>
+  <si>
+    <t>32 Position FFC, FPC Connector Contacts, Bottom 0.020 (0.50mm) Surface Mount, Right Angle</t>
+  </si>
+  <si>
+    <t>15 Position Receptacle, Pass Through Connector 0.100 (2.54mm) Surface Mount Gold</t>
+  </si>
+  <si>
+    <t>6 Position Receptacle, Pass Through Connector 0.100 (2.54mm) Surface Mount Gold</t>
+  </si>
+  <si>
+    <t>Connector Header Surface Mount, Right Angle 4 position 0.039 (1.00mm)</t>
+  </si>
+  <si>
+    <t>Total (USD)</t>
+  </si>
+  <si>
+    <t>Unit Price (USD)</t>
+  </si>
+  <si>
+    <t>TSTICKTOUCH</t>
+  </si>
+  <si>
+    <t>TOUCHBOARD</t>
+  </si>
+  <si>
+    <t>T-Stick Touch board (assembly + fabrication)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="\$0.000"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -660,6 +734,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -842,7 +921,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1005,6 +1084,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1052,7 +1157,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1072,22 +1177,10 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="16" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1100,6 +1193,34 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1456,11 +1577,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G57"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1471,21 +1592,21 @@
     <col min="4" max="4" width="27.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="61.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="45" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" style="17" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+    </row>
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>73</v>
       </c>
@@ -1504,11 +1625,14 @@
       <c r="F2" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="9" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H2" s="21" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>35</v>
       </c>
@@ -1527,9 +1651,15 @@
       <c r="F3" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G3" s="14"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G3" s="18">
+        <f>H3*C3</f>
+        <v>6.9589999999999996</v>
+      </c>
+      <c r="H3" s="18">
+        <v>6.9589999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>78</v>
       </c>
@@ -1548,9 +1678,15 @@
       <c r="F4" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G4" s="14"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G4" s="18">
+        <f t="shared" ref="G4:G30" si="0">H4*C4</f>
+        <v>2.1480000000000001</v>
+      </c>
+      <c r="H4" s="18">
+        <v>2.1480000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>78</v>
       </c>
@@ -1569,9 +1705,15 @@
       <c r="F5" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G5" s="14"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G5" s="18">
+        <f t="shared" si="0"/>
+        <v>1.98</v>
+      </c>
+      <c r="H5" s="18">
+        <v>1.98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>83</v>
       </c>
@@ -1590,9 +1732,15 @@
       <c r="F6" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G6" s="14"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G6" s="18">
+        <f t="shared" si="0"/>
+        <v>0.12</v>
+      </c>
+      <c r="H6" s="18">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>86</v>
       </c>
@@ -1611,9 +1759,15 @@
       <c r="F7" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G7" s="14"/>
-    </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G7" s="18">
+        <f t="shared" si="0"/>
+        <v>0.54200000000000004</v>
+      </c>
+      <c r="H7" s="18">
+        <v>0.27100000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>81</v>
       </c>
@@ -1632,9 +1786,15 @@
       <c r="F8" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G8" s="14"/>
-    </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G8" s="18">
+        <f t="shared" si="0"/>
+        <v>9.3539999999999992</v>
+      </c>
+      <c r="H8" s="18">
+        <v>9.3539999999999992</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>80</v>
       </c>
@@ -1653,9 +1813,15 @@
       <c r="F9" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G9" s="14"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G9" s="18">
+        <f t="shared" si="0"/>
+        <v>1.1579999999999999</v>
+      </c>
+      <c r="H9" s="18">
+        <v>1.1579999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>77</v>
       </c>
@@ -1674,9 +1840,15 @@
       <c r="F10" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="14"/>
-    </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G10" s="18">
+        <f t="shared" si="0"/>
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="H10" s="18">
+        <v>0.58199999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>74</v>
       </c>
@@ -1695,9 +1867,15 @@
       <c r="F11" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G11" s="14"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G11" s="18">
+        <f t="shared" si="0"/>
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="H11" s="18">
+        <v>0.79600000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>74</v>
       </c>
@@ -1716,9 +1894,15 @@
       <c r="F12" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G12" s="14"/>
-    </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G12" s="18">
+        <f t="shared" si="0"/>
+        <v>0.42599999999999999</v>
+      </c>
+      <c r="H12" s="18">
+        <v>0.21299999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>74</v>
       </c>
@@ -1737,9 +1921,15 @@
       <c r="F13" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G13" s="14"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G13" s="18">
+        <f t="shared" si="0"/>
+        <v>0.66400000000000003</v>
+      </c>
+      <c r="H13" s="18">
+        <v>0.33200000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>76</v>
       </c>
@@ -1758,9 +1948,15 @@
       <c r="F14" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G14" s="14"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G14" s="18">
+        <f t="shared" si="0"/>
+        <v>0.76600000000000001</v>
+      </c>
+      <c r="H14" s="18">
+        <v>0.76600000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>82</v>
       </c>
@@ -1779,9 +1975,15 @@
       <c r="F15" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G15" s="14"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G15" s="18">
+        <f t="shared" si="0"/>
+        <v>0.69399999999999995</v>
+      </c>
+      <c r="H15" s="18">
+        <v>0.69399999999999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>88</v>
       </c>
@@ -1800,9 +2002,15 @@
       <c r="F16" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G16" s="14"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G16" s="18">
+        <f t="shared" si="0"/>
+        <v>1.218</v>
+      </c>
+      <c r="H16" s="18">
+        <v>1.218</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>89</v>
       </c>
@@ -1821,9 +2029,15 @@
       <c r="F17" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G17" s="14"/>
-    </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G17" s="18">
+        <f t="shared" si="0"/>
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="H17" s="18">
+        <v>0.88200000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>85</v>
       </c>
@@ -1842,9 +2056,15 @@
       <c r="F18" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G18" s="14"/>
-    </row>
-    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G18" s="18">
+        <f t="shared" si="0"/>
+        <v>1.2350000000000001</v>
+      </c>
+      <c r="H18" s="18">
+        <v>1.2350000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>84</v>
       </c>
@@ -1863,9 +2083,15 @@
       <c r="F19" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G19" s="14"/>
-    </row>
-    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G19" s="18">
+        <f t="shared" si="0"/>
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="H19" s="18">
+        <v>4.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>84</v>
       </c>
@@ -1884,9 +2110,15 @@
       <c r="F20" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G20" s="14"/>
-    </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G20" s="18">
+        <f t="shared" si="0"/>
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="H20" s="18">
+        <v>4.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>84</v>
       </c>
@@ -1905,9 +2137,15 @@
       <c r="F21" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G21" s="14"/>
-    </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G21" s="18">
+        <f t="shared" si="0"/>
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="H21" s="18">
+        <v>4.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>84</v>
       </c>
@@ -1926,9 +2164,15 @@
       <c r="F22" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G22" s="14"/>
-    </row>
-    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G22" s="18">
+        <f t="shared" si="0"/>
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="H22" s="18">
+        <v>6.9000000000000006E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>84</v>
       </c>
@@ -1947,9 +2191,15 @@
       <c r="F23" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G23" s="14"/>
-    </row>
-    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G23" s="18">
+        <f t="shared" si="0"/>
+        <v>0.23399999999999999</v>
+      </c>
+      <c r="H23" s="18">
+        <v>3.9E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>84</v>
       </c>
@@ -1968,9 +2218,15 @@
       <c r="F24" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G24" s="14"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G24" s="18">
+        <f t="shared" si="0"/>
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="H24" s="18">
+        <v>6.9000000000000006E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>75</v>
       </c>
@@ -1989,9 +2245,15 @@
       <c r="F25" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G25" s="14"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G25" s="18">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="H25" s="18">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>75</v>
       </c>
@@ -2010,9 +2272,15 @@
       <c r="F26" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G26" s="14"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G26" s="18">
+        <f t="shared" si="0"/>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="H26" s="18">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>75</v>
       </c>
@@ -2031,9 +2299,15 @@
       <c r="F27" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G27" s="14"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G27" s="18">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="H27" s="18">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>75</v>
       </c>
@@ -2052,9 +2326,15 @@
       <c r="F28" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G28" s="14"/>
-    </row>
-    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G28" s="18">
+        <f t="shared" si="0"/>
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="H28" s="18">
+        <v>0.13900000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>79</v>
       </c>
@@ -2073,9 +2353,15 @@
       <c r="F29" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G29" s="14"/>
-    </row>
-    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G29" s="18">
+        <f t="shared" si="0"/>
+        <v>7.2279999999999998</v>
+      </c>
+      <c r="H29" s="18">
+        <v>7.2279999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>87</v>
       </c>
@@ -2094,9 +2380,15 @@
       <c r="F30" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G30" s="14"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G30" s="18">
+        <f t="shared" si="0"/>
+        <v>1.151</v>
+      </c>
+      <c r="H30" s="18">
+        <v>1.151</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>126</v>
       </c>
@@ -2115,424 +2407,638 @@
       <c r="F31" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G31" s="14"/>
-    </row>
-    <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F32" s="8" t="s">
+      <c r="G31" s="10">
+        <f>(30+88)/5</f>
+        <v>23.6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="22"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="G32" s="11">
+        <f>SUM(G3:G31)</f>
+        <v>62.885999999999996</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F33" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="G32" s="15">
-        <f>1.3*SUM(G3:G31)</f>
+      <c r="G33" s="11">
+        <f>1.3*G32</f>
+        <v>81.751800000000003</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F34" s="19"/>
+      <c r="G34" s="12"/>
+    </row>
+    <row r="35" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A35" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="B35" s="20"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20"/>
+    </row>
+    <row r="36" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A34" s="9" t="s">
+      <c r="D36" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="H36" s="23" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C37" s="3">
+        <v>1</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="G37" s="10">
+        <f>C37*H37</f>
+        <v>2.5760000000000001</v>
+      </c>
+      <c r="H37" s="18">
+        <v>2.5760000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C38" s="3">
+        <v>2</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="G38" s="10">
+        <f t="shared" ref="G38:G40" si="1">C38*H38</f>
+        <v>10.773999999999999</v>
+      </c>
+      <c r="H38" s="18">
+        <v>5.3869999999999996</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C39" s="3">
+        <v>1</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="G39" s="10">
+        <f t="shared" si="1"/>
+        <v>2.5590000000000002</v>
+      </c>
+      <c r="H39" s="18">
+        <v>2.5590000000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C40" s="3">
+        <v>4</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="G40" s="10">
+        <f t="shared" si="1"/>
+        <v>1.1759999999999999</v>
+      </c>
+      <c r="H40" s="18">
+        <v>0.29399999999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C41" s="3">
+        <v>1</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="G41" s="10">
+        <f>(30+5)/5</f>
+        <v>7</v>
+      </c>
+      <c r="H41" s="24"/>
+    </row>
+    <row r="42" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F42" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="G42" s="11">
+        <f>SUM(G37:G41)</f>
+        <v>24.084999999999997</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F43" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="G43" s="10">
+        <f>G42*1.3</f>
+        <v>31.310499999999998</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F44" s="19"/>
+    </row>
+    <row r="45" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A45" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+      <c r="B45" s="20"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="20"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B46" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C46" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E35" s="3" t="s">
+      <c r="D46" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E46" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="F46" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="G35" s="13" t="s">
+      <c r="G46" s="9" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+    <row r="47" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B47" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C47" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E36" s="3" t="s">
+      <c r="D47" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E47" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="F36" s="5" t="s">
+      <c r="F47" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="G36" s="14">
+      <c r="G47" s="10">
         <f>19*1.3</f>
         <v>24.7</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+    <row r="48" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B48" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="C37" s="3">
-        <v>1</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E37" s="3" t="s">
+      <c r="C48" s="3">
+        <v>1</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E48" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="F37" s="5" t="s">
+      <c r="F48" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="G37" s="14">
+      <c r="G48" s="10">
         <v>16.32</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+    <row r="49" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B49" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C38" s="3">
-        <v>1</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E38" s="3" t="s">
+      <c r="C49" s="3">
+        <v>1</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E49" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="F38" s="5" t="s">
+      <c r="F49" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="G38" s="14">
+      <c r="G49" s="10">
         <v>26.13</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E39" s="3" t="s">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E50" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="F39" s="5"/>
-      <c r="G39" s="14"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E40" s="3" t="s">
+      <c r="F50" s="5"/>
+      <c r="G50" s="10"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="3"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E51" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="F40" s="3"/>
-      <c r="G40" s="14"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E41" s="3" t="s">
+      <c r="F51" s="3"/>
+      <c r="G51" s="10"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="3"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E52" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="F41" s="3"/>
-      <c r="G41" s="14"/>
-    </row>
-    <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F42" s="8" t="s">
+      <c r="F52" s="3"/>
+      <c r="G52" s="10"/>
+    </row>
+    <row r="53" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F53" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="G42" s="14">
-        <f>SUM(G36:G41)</f>
+      <c r="G53" s="10">
+        <f>SUM(G47:G52)</f>
         <v>67.149999999999991</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F43" s="11"/>
-      <c r="G43" s="16"/>
-    </row>
-    <row r="44" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A44" s="7" t="s">
+    <row r="54" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F54" s="8"/>
+      <c r="G54" s="12"/>
+    </row>
+    <row r="55" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A55" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="B44" s="7"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="s">
+      <c r="B55" s="15"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="15"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B56" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C56" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D45" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E45" s="6" t="s">
+      <c r="D56" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E56" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F45" s="6" t="s">
+      <c r="F56" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="G45" s="13" t="s">
+      <c r="G56" s="9" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
+    <row r="57" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B46" s="12" t="s">
+      <c r="B57" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C46" s="3">
+      <c r="C57" s="3">
         <v>2</v>
       </c>
-      <c r="D46" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E46" s="3" t="s">
+      <c r="D57" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E57" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="F57" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="G46" s="18">
+      <c r="G57" s="14">
         <v>1.6</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
+    <row r="58" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B47" s="4">
+      <c r="B58" s="4">
         <v>5384</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C58" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E47" s="3" t="s">
+      <c r="D58" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E58" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="F58" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="G47" s="14">
+      <c r="G58" s="10">
         <v>2.1</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+    <row r="59" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B48" s="4">
+      <c r="B59" s="4">
         <v>1862</v>
       </c>
-      <c r="C48" s="3">
-        <v>1</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E48" s="3" t="s">
+      <c r="C59" s="3">
+        <v>1</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E59" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="F48" s="5" t="s">
+      <c r="F59" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="G48" s="14">
+      <c r="G59" s="10">
         <v>1.5</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
+    <row r="60" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B49" s="4">
+      <c r="B60" s="4">
         <v>4714</v>
       </c>
-      <c r="C49" s="3">
-        <v>1</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E49" s="3" t="s">
+      <c r="C60" s="3">
+        <v>1</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E60" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="F49" s="5" t="s">
+      <c r="F60" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="G49" s="14">
+      <c r="G60" s="10">
         <v>0.95</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
+    <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B50" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C50" s="3">
-        <v>1</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E50" s="3" t="s">
+      <c r="B61" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C61" s="3">
+        <v>1</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E61" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="F50" s="2" t="s">
+      <c r="F61" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="G50" s="14">
+      <c r="G61" s="10">
         <f>6/1.3</f>
         <v>4.615384615384615</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
+    <row r="62" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B62" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C51" s="3">
-        <v>1</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E51" s="3" t="s">
+      <c r="C62" s="3">
+        <v>1</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E62" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="F51" s="5" t="s">
+      <c r="F62" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="G51" s="14">
+      <c r="G62" s="10">
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
+    <row r="63" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B63" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E52" s="3" t="s">
+      <c r="C63" s="3">
+        <v>1</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E63" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="F52" s="5" t="s">
+      <c r="F63" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="G52" s="14">
+      <c r="G63" s="10">
         <v>105.94</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="3"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E53" s="3" t="s">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="3"/>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E64" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="F53" s="3"/>
-      <c r="G53" s="14"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="3"/>
-      <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E54" s="3" t="s">
+      <c r="F64" s="3"/>
+      <c r="G64" s="10"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="3"/>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E65" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="F54" s="3"/>
-      <c r="G54" s="14"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="3"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E55" s="3" t="s">
+      <c r="F65" s="3"/>
+      <c r="G65" s="10"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="3"/>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E66" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F55" s="3"/>
-      <c r="G55" s="14"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="3"/>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E56" s="3" t="s">
+      <c r="F66" s="3"/>
+      <c r="G66" s="10"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="3"/>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E67" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="F56" s="3"/>
-      <c r="G56" s="14"/>
-    </row>
-    <row r="57" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F57" s="8" t="s">
+      <c r="F67" s="3"/>
+      <c r="G67" s="10"/>
+    </row>
+    <row r="68" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F68" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="G57" s="14">
-        <f>1.3*SUM(G46:G56)</f>
+      <c r="G68" s="10">
+        <f>1.3*SUM(G57:G67)</f>
         <v>153.21199999999999</v>
       </c>
     </row>
@@ -2540,22 +3046,23 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:E30">
     <sortCondition ref="A2:A30"/>
   </sortState>
-  <mergeCells count="3">
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A34:G34"/>
+  <mergeCells count="4">
+    <mergeCell ref="A55:F55"/>
+    <mergeCell ref="A45:G45"/>
     <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A35:G35"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F36" r:id="rId1"/>
-    <hyperlink ref="F51" r:id="rId2" display="https://www.sparkfun.com/products/12899"/>
-    <hyperlink ref="F48" r:id="rId3" display="https://www.adafruit.com/product/1862"/>
-    <hyperlink ref="F49" r:id="rId4" display="https://www.adafruit.com/product/4714"/>
-    <hyperlink ref="F46" r:id="rId5" display="https://www.sparkfun.com/products/17258"/>
-    <hyperlink ref="F47" r:id="rId6" display="https://www.sparkfun.com/products/17257"/>
-    <hyperlink ref="F50" r:id="rId7" display="https://18650canada.ca/product/18650-rechargeable-battery/"/>
-    <hyperlink ref="F52" r:id="rId8"/>
-    <hyperlink ref="F37" r:id="rId9" display="https://www.digikey.ca/en/products/detail/interlink-electronics/34-00158/16803578"/>
-    <hyperlink ref="F38" r:id="rId10" display="https://www.digikey.ca/en/products/detail/interlink-electronics/34-00120/16803577"/>
+    <hyperlink ref="F47" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F62" r:id="rId2" display="https://www.sparkfun.com/products/12899" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F59" r:id="rId3" display="https://www.adafruit.com/product/1862" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="F60" r:id="rId4" display="https://www.adafruit.com/product/4714" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="F57" r:id="rId5" display="https://www.sparkfun.com/products/17258" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="F58" r:id="rId6" display="https://www.sparkfun.com/products/17257" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="F61" r:id="rId7" display="https://18650canada.ca/product/18650-rechargeable-battery/" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="F63" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="F48" r:id="rId9" display="https://www.digikey.ca/en/products/detail/interlink-electronics/34-00158/16803578" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="F49" r:id="rId10" display="https://www.digikey.ca/en/products/detail/interlink-electronics/34-00120/16803577" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId11"/>

</xml_diff>